<commit_message>
Added some more datasets, added README and gitignore
</commit_message>
<xml_diff>
--- a/reference.xlsx
+++ b/reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicvphq/Desktop/kaggle-csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D215E407-2484-1843-BBC7-235DB2817313}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBB6B2F-D953-0E4B-82E9-4588BA617985}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="8020" windowWidth="39760" windowHeight="18120" xr2:uid="{26746F1A-DB84-DF4C-BF9D-060F66A10C37}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -235,6 +235,48 @@
   </si>
   <si>
     <t>https://www.kaggle.com/mylesoneill/game-of-thrones</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/abecklas/fifa-world-cup</t>
+  </si>
+  <si>
+    <t>FIFA World Cup</t>
+  </si>
+  <si>
+    <t>All the results from World cups</t>
+  </si>
+  <si>
+    <t>WorldCupMatches</t>
+  </si>
+  <si>
+    <t>student-por</t>
+  </si>
+  <si>
+    <t>student-mat</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/uciml/student-alcohol-consumption</t>
+  </si>
+  <si>
+    <t>Student Alcohol Consumption</t>
+  </si>
+  <si>
+    <t>Social, gender and study data from secondary school students (portugese)</t>
+  </si>
+  <si>
+    <t>Social, gender and study data from secondary school students (math)</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/rtatman/chocolate-bar-ratings</t>
+  </si>
+  <si>
+    <t>flavors_of_cacao</t>
+  </si>
+  <si>
+    <t>Chocolate Bar Ratings</t>
+  </si>
+  <si>
+    <t>Expert ratings of over 1,700 chocolate bars</t>
   </si>
 </sst>
 </file>
@@ -614,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A0AC3E-9746-1C41-923F-C79D5509804B}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,6 +979,62 @@
         <v>69</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more datasets, mvoed data into data folder
</commit_message>
<xml_diff>
--- a/reference.xlsx
+++ b/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicvphq/Desktop/kaggle-csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBB6B2F-D953-0E4B-82E9-4588BA617985}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A046376C-05F8-334B-9423-1179F0E97F12}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="8020" windowWidth="39760" windowHeight="18120" xr2:uid="{26746F1A-DB84-DF4C-BF9D-060F66A10C37}"/>
+    <workbookView xWindow="17600" yWindow="8140" windowWidth="39760" windowHeight="11840" xr2:uid="{26746F1A-DB84-DF4C-BF9D-060F66A10C37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
   <si>
     <t>name</t>
   </si>
@@ -277,14 +277,142 @@
   </si>
   <si>
     <t>Expert ratings of over 1,700 chocolate bars</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/harlfoxem/housesalesprediction</t>
+  </si>
+  <si>
+    <t>kc_house_data</t>
+  </si>
+  <si>
+    <t>House Sales in King County, USA</t>
+  </si>
+  <si>
+    <t>Housing price data from KC, USA</t>
+  </si>
+  <si>
+    <t>Default of Credit Card Clients Dataset</t>
+  </si>
+  <si>
+    <t>Default Payments of Credit Card Clients in Taiwan from 2005</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/uciml/default-of-credit-card-clients-dataset</t>
+  </si>
+  <si>
+    <t>UCI_Credit_Card</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/rajanand/key-indicators-of-annual-health-survey</t>
+  </si>
+  <si>
+    <t>Key_indicator_districtwise</t>
+  </si>
+  <si>
+    <t>Health Analytics</t>
+  </si>
+  <si>
+    <t>26 health indicators (642 variables) from 284 districts of India</t>
+  </si>
+  <si>
+    <t>Fatal Police Shootings in the US</t>
+  </si>
+  <si>
+    <t>Fatal police shootings in the US since 2015 with additional US census data</t>
+  </si>
+  <si>
+    <t>MedianHouseholdIncome2015</t>
+  </si>
+  <si>
+    <t>PercentagePeopleBelowPovertyLevel</t>
+  </si>
+  <si>
+    <t>PercentOver25CompletedHighSchool</t>
+  </si>
+  <si>
+    <t>PoliceKillingsUS</t>
+  </si>
+  <si>
+    <t>ShareRaceByCity</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/kwullum/fatal-police-shootings-in-the-us</t>
+  </si>
+  <si>
+    <t>Social Power NBA</t>
+  </si>
+  <si>
+    <t>NBA on the court performance with Social Influence, Popularity and Power</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/noahgift/social-power-nba</t>
+  </si>
+  <si>
+    <t>nba_2017_elo</t>
+  </si>
+  <si>
+    <t>nba_2017_endorsements</t>
+  </si>
+  <si>
+    <t>nba_2017_team_valuations</t>
+  </si>
+  <si>
+    <t>Celebrity Deaths</t>
+  </si>
+  <si>
+    <t>All wikipedia-listed celebrity deaths from 2006</t>
+  </si>
+  <si>
+    <t>celebrity_deaths_4</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/hugodarwood/celebrity-deaths</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/nasa/meteorite-landings</t>
+  </si>
+  <si>
+    <t>Meteorite Landings</t>
+  </si>
+  <si>
+    <t>Data on over 45k meteorites that have struck Earth</t>
+  </si>
+  <si>
+    <t>meteorite-landings</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/the-guardian/olympic-games</t>
+  </si>
+  <si>
+    <t>summer</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>Olympic Sports and Medals, 1896-2014</t>
+  </si>
+  <si>
+    <t>Which countries and athletes have won the most medals at the Olympic games? (summer)</t>
+  </si>
+  <si>
+    <t>Which countries and athletes have won the most medals at the Olympic games? (winter)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -298,6 +426,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -336,12 +470,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,284 +792,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A0AC3E-9746-1C41-923F-C79D5509804B}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="112" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="58.5" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="70.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -944,7 +1080,7 @@
       <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D20" t="s">
@@ -958,7 +1094,7 @@
       <c r="B21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D21" t="s">
@@ -972,7 +1108,7 @@
       <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D22" t="s">
@@ -1033,6 +1169,216 @@
       </c>
       <c r="D26" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed a csv title in data
</commit_message>
<xml_diff>
--- a/reference.xlsx
+++ b/reference.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicvphq/Desktop/gh-repos/kaggle-csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\kaggle-csv-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD7345B-2E98-1E4B-B97D-B8347F015A29}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="4840" windowWidth="31800" windowHeight="16540" xr2:uid="{26746F1A-DB84-DF4C-BF9D-060F66A10C37}"/>
+    <workbookView xWindow="6563" yWindow="5378" windowWidth="31800" windowHeight="16538"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -642,9 +641,6 @@
     <t>https://www.kaggle.com/fernandol/countries-of-the-world</t>
   </si>
   <si>
-    <t>countries of the world</t>
-  </si>
-  <si>
     <t>Countries of the World</t>
   </si>
   <si>
@@ -730,13 +726,16 @@
   </si>
   <si>
     <t>Game related data for NBA players since 1950</t>
+  </si>
+  <si>
+    <t>countries_of_the_world</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1094,23 +1093,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A0AC3E-9746-1C41-923F-C79D5509804B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45" style="3" customWidth="1"/>
-    <col min="2" max="2" width="71.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="71.1875" style="3" customWidth="1"/>
     <col min="3" max="3" width="24" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="70.1875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.8125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1124,10 +1123,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1143,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1177,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1228,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>64</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
         <v>77</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
         <v>77</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
         <v>86</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>88</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
         <v>94</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
         <v>96</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
         <v>96</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
         <v>96</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>96</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
         <v>104</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
         <v>104</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
         <v>110</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
         <v>121</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>121</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
         <v>126</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>129</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
         <v>129</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
         <v>129</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
         <v>129</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
         <v>129</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
         <v>129</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
         <v>129</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
         <v>129</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
         <v>129</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
         <v>129</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
         <v>129</v>
       </c>
@@ -2028,7 +2027,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
         <v>129</v>
       </c>
@@ -2045,7 +2044,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
         <v>129</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
         <v>129</v>
       </c>
@@ -2079,7 +2078,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
         <v>129</v>
       </c>
@@ -2096,7 +2095,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
         <v>148</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
         <v>153</v>
       </c>
@@ -2130,7 +2129,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
         <v>155</v>
       </c>
@@ -2147,7 +2146,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
         <v>157</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
         <v>157</v>
       </c>
@@ -2181,7 +2180,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
         <v>166</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
         <v>170</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
         <v>173</v>
       </c>
@@ -2232,7 +2231,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
         <v>178</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
         <v>183</v>
       </c>
@@ -2266,7 +2265,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
         <v>183</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
         <v>187</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
         <v>189</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
         <v>193</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
         <v>193</v>
       </c>
@@ -2351,7 +2350,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
         <v>193</v>
       </c>
@@ -2368,7 +2367,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
         <v>193</v>
       </c>
@@ -2385,7 +2384,7 @@
         <v>20190201</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
         <v>202</v>
       </c>
@@ -2402,15 +2401,15 @@
         <v>20190204</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="C77" s="3" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>204</v>
@@ -2419,137 +2418,137 @@
         <v>20190204</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="E78" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="E79" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E80" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="C81" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="E81" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>223</v>
-      </c>
       <c r="C82" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="E82" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="D83" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E83" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E84" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E85" s="3">
         <v>20190204</v>

</xml_diff>

<commit_message>
Added some R datasets
</commit_message>
<xml_diff>
--- a/reference.xlsx
+++ b/reference.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\kaggle-csv-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\dc-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6563" yWindow="5378" windowWidth="31800" windowHeight="16538"/>
+    <workbookView xWindow="6563" yWindow="5918" windowWidth="31800" windowHeight="16538"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="252">
   <si>
     <t>name</t>
   </si>
@@ -729,13 +729,64 @@
   </si>
   <si>
     <t>countries_of_the_world</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>BEPS</t>
+  </si>
+  <si>
+    <t>These data are drawn from the 1997-2001 British Election Panel Study (BEPS).</t>
+  </si>
+  <si>
+    <t>British Election Panel Study</t>
+  </si>
+  <si>
+    <t>https://vincentarelbundock.github.io/Rdatasets/datasets.html</t>
+  </si>
+  <si>
+    <t>KosteckiDillon</t>
+  </si>
+  <si>
+    <t>Subset of data on migraine treatments collected by Tammy Kostecki-Dillon.</t>
+  </si>
+  <si>
+    <t>Treatment of Migraine Headaches</t>
+  </si>
+  <si>
+    <t>mpg</t>
+  </si>
+  <si>
+    <t>Fuel economy data from 1999 and 2008 for 38 popular models of car</t>
+  </si>
+  <si>
+    <t>MPG</t>
+  </si>
+  <si>
+    <t>diamonds</t>
+  </si>
+  <si>
+    <t>Prices of 50,000 round cut diamonds</t>
+  </si>
+  <si>
+    <t>Diamonds</t>
+  </si>
+  <si>
+    <t>Data from a clinical trial comparing two treatments for a respiratory illness</t>
+  </si>
+  <si>
+    <t>Respitory</t>
+  </si>
+  <si>
+    <t>respitory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -753,6 +804,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="VIC"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -775,11 +832,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,1467 +1152,1581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="45" style="3" customWidth="1"/>
-    <col min="2" max="2" width="71.1875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.1875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.8125" style="3"/>
+    <col min="1" max="1" width="10.8125" style="3"/>
+    <col min="2" max="2" width="45" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.1875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24" style="3" customWidth="1"/>
+    <col min="5" max="5" width="70.1875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.8125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="17.649999999999999">
+      <c r="B2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.649999999999999">
+      <c r="B3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.649999999999999">
+      <c r="B4" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.649999999999999">
+      <c r="B5" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F5" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17.649999999999999">
+      <c r="B6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="F7" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="F8" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
+      <c r="F9" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="F10" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
+      <c r="F11" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+      <c r="F12" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
+      <c r="F13" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
+      <c r="F14" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
+      <c r="F15" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
+      <c r="F16" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
+      <c r="F17" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
+      <c r="F18" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
+      <c r="F19" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
+      <c r="F20" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
+      <c r="F21" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
+      <c r="F22" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
+      <c r="F23" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
+      <c r="F24" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
+      <c r="F25" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
+      <c r="F26" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
+      <c r="F27" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2" t="s">
+      <c r="F28" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
+      <c r="F29" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
+      <c r="F30" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
+      <c r="F31" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
+      <c r="F32" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
+      <c r="F33" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
+      <c r="F34" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
+      <c r="F35" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="3">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
+      <c r="F36" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="3">
+        <v>1</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
+      <c r="F37" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="3">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2" t="s">
+      <c r="F38" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2" t="s">
+      <c r="F39" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
+      <c r="F40" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
+      <c r="F41" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E37" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
+      <c r="F42" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
+      <c r="F43" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
+      <c r="F44" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
+      <c r="F45" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="B46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
+      <c r="F46" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
+      <c r="F47" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="B48" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
+      <c r="F48" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="B49" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
+      <c r="F49" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="B50" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="2" t="s">
+      <c r="F50" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="B51" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E46" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
+      <c r="F51" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="B52" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="2" t="s">
+      <c r="F52" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E48" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2" t="s">
+      <c r="F53" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="B54" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2" t="s">
+      <c r="F54" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="B55" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2" t="s">
+      <c r="F55" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="B56" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2" t="s">
+      <c r="F56" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="B57" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E52" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="2" t="s">
+      <c r="F57" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="B58" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E53" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="2" t="s">
+      <c r="F58" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="B59" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="2" t="s">
+      <c r="F59" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="B60" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E55" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="2" t="s">
+      <c r="F60" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="B61" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E56" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
+      <c r="F61" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="B62" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E57" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="2" t="s">
+      <c r="F62" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="B63" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E58" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="2" t="s">
+      <c r="F63" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="3">
+        <v>1</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E59" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="2" t="s">
+      <c r="F64" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="B65" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E60" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="3" t="s">
+      <c r="F65" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="B66" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E61" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="3" t="s">
+      <c r="F66" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="B67" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E62" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="3" t="s">
+      <c r="F67" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E63" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="3" t="s">
+      <c r="F68" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="3">
+        <v>1</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E64" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="3" t="s">
+      <c r="F69" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="B70" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E65" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="3" t="s">
+      <c r="F70" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="B71" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E66" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="3" t="s">
+      <c r="F71" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="B72" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E67" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="3" t="s">
+      <c r="F72" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="B73" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E68" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="3" t="s">
+      <c r="F73" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="B74" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E69" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="3" t="s">
+      <c r="F74" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="B75" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E70" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="3" t="s">
+      <c r="F75" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="3">
+        <v>1</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E71" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="3" t="s">
+      <c r="F76" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="B77" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E72" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="3" t="s">
+      <c r="F77" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="B78" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E73" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="3" t="s">
+      <c r="F78" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="B79" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E74" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="3" t="s">
+      <c r="F79" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="B80" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="D80" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="E80" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E75" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="3" t="s">
+      <c r="F80" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E76" s="3">
+      <c r="F81" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="3" t="s">
+    <row r="82" spans="2:6">
+      <c r="B82" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C82" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E77" s="3">
+      <c r="F82" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="3" t="s">
+    <row r="83" spans="2:6">
+      <c r="B83" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E78" s="3">
+      <c r="F83" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="3" t="s">
+    <row r="84" spans="2:6">
+      <c r="B84" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E79" s="3">
+      <c r="F84" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="3" t="s">
+    <row r="85" spans="2:6">
+      <c r="B85" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E80" s="3">
+      <c r="F85" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="3" t="s">
+    <row r="86" spans="2:6">
+      <c r="B86" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E81" s="3">
+      <c r="F86" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="3" t="s">
+    <row r="87" spans="2:6">
+      <c r="B87" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="D87" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="E87" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E82" s="3">
+      <c r="F87" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="3" t="s">
+    <row r="88" spans="2:6">
+      <c r="B88" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E83" s="3">
+      <c r="F88" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="3" t="s">
+    <row r="89" spans="2:6">
+      <c r="B89" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E84" s="3">
+      <c r="F89" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="3" t="s">
+    <row r="90" spans="2:6">
+      <c r="B90" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E85" s="3">
+      <c r="F90" s="3">
         <v>20190204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more R datasetrs
</commit_message>
<xml_diff>
--- a/reference.xlsx
+++ b/reference.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6563" yWindow="5918" windowWidth="31800" windowHeight="16538"/>
+    <workbookView xWindow="6563" yWindow="6458" windowWidth="31800" windowHeight="16538" tabRatio="342"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="292">
   <si>
     <t>name</t>
   </si>
@@ -780,13 +780,133 @@
   </si>
   <si>
     <t>respitory</t>
+  </si>
+  <si>
+    <t>Airbag and other influences on accident fatalities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nassCDS </t>
+  </si>
+  <si>
+    <t>Cyber Security Breaches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breaches </t>
+  </si>
+  <si>
+    <t>Daily Observations on Exchange Rates of the US Dollar Against Other Currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garch </t>
+  </si>
+  <si>
+    <t>Cybersecurity breaches reported to the US Department of Health and Human Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HHSCyberSecurityBreaches </t>
+  </si>
+  <si>
+    <t>US fatal road accident data for automobiles, 1998 to 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FARS </t>
+  </si>
+  <si>
+    <t>A study of Parkinson's disease and APOE, LRRK2, SNCA makers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD </t>
+  </si>
+  <si>
+    <t>State Anxiety data from the PMC lab over multiple occasions.</t>
+  </si>
+  <si>
+    <t>tai</t>
+  </si>
+  <si>
+    <t>75 mood items from the Motivational State Questionnaire for 3032 unique participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msqR </t>
+  </si>
+  <si>
+    <t>Eysenck Personality Inventory (EPI) data for 3570 participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epiR </t>
+  </si>
+  <si>
+    <t>1992 United Kingdom electoral returns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKHouseOfCommons </t>
+  </si>
+  <si>
+    <t>Yearly batting records for all major league baseball players</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baseball </t>
+  </si>
+  <si>
+    <t>Biopsy Data on Breast Cancer Patients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biopsy </t>
+  </si>
+  <si>
+    <t>The Forbes 2000 Ranking of the World's Biggest Companies (Year 2004)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forbes2000 </t>
+  </si>
+  <si>
+    <t>Housing sales in TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txhousing </t>
+  </si>
+  <si>
+    <t>Airbags</t>
+  </si>
+  <si>
+    <t>USD Exchange Rates</t>
+  </si>
+  <si>
+    <t>Breaches</t>
+  </si>
+  <si>
+    <t>US Road Fatalities</t>
+  </si>
+  <si>
+    <t>Parkinsons</t>
+  </si>
+  <si>
+    <t>Anxiety Data</t>
+  </si>
+  <si>
+    <t>Mood</t>
+  </si>
+  <si>
+    <t>EPI</t>
+  </si>
+  <si>
+    <t>Baseball</t>
+  </si>
+  <si>
+    <t>Breast Cancer Biopsy</t>
+  </si>
+  <si>
+    <t>Forbes</t>
+  </si>
+  <si>
+    <t>Housing Texas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -811,6 +931,53 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="VIC"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="VIC"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="VIC"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="VIC"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -832,12 +999,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1152,51 +1331,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" activeCellId="1" sqref="B16 C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="47.0625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.8125" style="3"/>
-    <col min="2" max="2" width="45" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.1875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.1875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8125" style="3"/>
+    <col min="1" max="2" width="47.0625" style="3"/>
+    <col min="3" max="3" width="90.0625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="47.0625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.649999999999999">
-      <c r="B2" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>251</v>
+    <row r="2" spans="1:6" ht="21">
+      <c r="A2" s="9"/>
+      <c r="B2" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>253</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>239</v>
@@ -1205,15 +1382,16 @@
         <v>20190207</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.649999999999999">
-      <c r="B3" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>246</v>
+    <row r="3" spans="1:6" ht="21">
+      <c r="A3" s="9"/>
+      <c r="B3" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>255</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>239</v>
@@ -1222,15 +1400,16 @@
         <v>20190207</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.649999999999999">
-      <c r="B4" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>243</v>
+    <row r="4" spans="1:6" ht="21">
+      <c r="A4" s="9"/>
+      <c r="B4" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>257</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>239</v>
@@ -1239,15 +1418,16 @@
         <v>20190207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.649999999999999">
-      <c r="B5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>240</v>
+    <row r="5" spans="1:6" ht="21">
+      <c r="A5" s="9"/>
+      <c r="B5" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>259</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>239</v>
@@ -1256,15 +1436,16 @@
         <v>20190207</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.649999999999999">
-      <c r="B6" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>236</v>
+    <row r="6" spans="1:6" ht="21">
+      <c r="A6" s="9"/>
+      <c r="B6" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>261</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>239</v>
@@ -1273,256 +1454,259 @@
         <v>20190207</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
+    <row r="7" spans="1:6" ht="21">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>239</v>
+      </c>
+      <c r="F7" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21">
+      <c r="A8" s="9"/>
+      <c r="B8" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>265</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>239</v>
+      </c>
+      <c r="F8" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21">
+      <c r="A9" s="9"/>
+      <c r="B9" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
+      <c r="B10" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F10" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
+      <c r="B11" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>271</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F11" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
+      <c r="B12" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>273</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>19</v>
+      <c r="B13" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>275</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
+      <c r="B14" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F14" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
+      <c r="B15" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>239</v>
+      </c>
+      <c r="F15" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="22.9">
+      <c r="B16" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+        <v>239</v>
+      </c>
+      <c r="F16" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="17.649999999999999">
       <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>248</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>246</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>239</v>
+      </c>
+      <c r="F17" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="17.649999999999999">
       <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>245</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>244</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>243</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+        <v>239</v>
+      </c>
+      <c r="F18" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="17.649999999999999">
       <c r="B19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>242</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
+        <v>239</v>
+      </c>
+      <c r="F19" s="1">
+        <v>20190207</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="17.649999999999999">
       <c r="B20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>238</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>236</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="3">
-        <v>20190201</v>
+        <v>239</v>
+      </c>
+      <c r="F20" s="1">
+        <v>20190207</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F21" s="3">
         <v>20190201</v>
@@ -1530,16 +1714,16 @@
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F22" s="3">
         <v>20190201</v>
@@ -1547,16 +1731,16 @@
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="F23" s="3">
         <v>20190201</v>
@@ -1564,16 +1748,16 @@
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3">
         <v>20190201</v>
@@ -1581,16 +1765,16 @@
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="F25" s="3">
         <v>20190201</v>
@@ -1598,16 +1782,16 @@
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="F26" s="3">
         <v>20190201</v>
@@ -1615,16 +1799,16 @@
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="F27" s="3">
         <v>20190201</v>
@@ -1632,16 +1816,16 @@
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="2" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F28" s="3">
         <v>20190201</v>
@@ -1649,16 +1833,16 @@
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="F29" s="3">
         <v>20190201</v>
@@ -1666,16 +1850,16 @@
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="F30" s="3">
         <v>20190201</v>
@@ -1683,16 +1867,16 @@
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="2" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="F31" s="3">
         <v>20190201</v>
@@ -1700,371 +1884,368 @@
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" s="2" t="s">
+      <c r="F46" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" s="2" t="s">
+      <c r="F47" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3">
+      <c r="F48" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="3">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="3">
+      <c r="F49" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="3">
         <v>1</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F36" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="3">
+      <c r="F50" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="3">
         <v>1</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="3">
+      <c r="F51" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="3">
         <v>1</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F38" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F40" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="B41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="B42" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F42" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="3">
-        <v>1</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F43" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="B44" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="B45" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F45" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="B46" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F46" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="B47" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F47" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="B48" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F48" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="B49" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F49" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="B50" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F50" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="B51" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="B52" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="F52" s="3">
         <v>20190201</v>
@@ -2072,16 +2253,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="B53" s="2" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="F53" s="3">
         <v>20190201</v>
@@ -2089,16 +2270,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="B54" s="2" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="F54" s="3">
         <v>20190201</v>
@@ -2106,16 +2287,16 @@
     </row>
     <row r="55" spans="1:6">
       <c r="B55" s="2" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="F55" s="3">
         <v>20190201</v>
@@ -2123,33 +2304,36 @@
     </row>
     <row r="56" spans="1:6">
       <c r="B56" s="2" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="F56" s="3">
         <v>20190201</v>
       </c>
     </row>
     <row r="57" spans="1:6">
+      <c r="A57" s="3">
+        <v>1</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="F57" s="3">
         <v>20190201</v>
@@ -2157,16 +2341,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="B58" s="2" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="F58" s="3">
         <v>20190201</v>
@@ -2174,16 +2358,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F59" s="3">
         <v>20190201</v>
@@ -2191,16 +2375,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="B60" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F60" s="3">
         <v>20190201</v>
@@ -2208,16 +2392,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="B61" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F61" s="3">
         <v>20190201</v>
@@ -2231,7 +2415,7 @@
         <v>130</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>128</v>
@@ -2248,7 +2432,7 @@
         <v>130</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>128</v>
@@ -2258,20 +2442,17 @@
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="3">
-        <v>1</v>
-      </c>
       <c r="B64" s="2" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="F64" s="3">
         <v>20190201</v>
@@ -2279,260 +2460,257 @@
     </row>
     <row r="65" spans="1:6">
       <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="B66" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="B67" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="B68" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F68" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="B69" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="B70" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F70" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="B71" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F71" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="B72" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F72" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="B73" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F73" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="B74" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="B75" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F75" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="B76" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F76" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="B77" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="3">
+        <v>1</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F78" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="B79" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E79" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="F65" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="B66" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F66" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="B67" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F67" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="B68" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F68" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="3">
-        <v>1</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F69" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="B70" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F70" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="B71" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F71" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="B72" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F72" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="B73" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F73" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="B74" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F74" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="B75" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F75" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="3">
-        <v>1</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F76" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="B77" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F77" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="B78" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F78" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="B79" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="F79" s="3">
         <v>20190201</v>
@@ -2540,188 +2718,432 @@
     </row>
     <row r="80" spans="1:6">
       <c r="B80" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F80" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="B81" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F81" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="B82" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F82" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="3">
+        <v>1</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F83" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="B84" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F84" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="B85" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F85" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="B86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F86" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="B87" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F87" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="B88" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F88" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="B89" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F89" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="3">
+        <v>1</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F90" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="B91" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D91" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F91" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="B92" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F92" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="B93" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F93" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="B94" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F80" s="3">
-        <v>20190201</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6">
-      <c r="B81" s="3" t="s">
+      <c r="F94" s="3">
+        <v>20190201</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="B95" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F81" s="3">
+      <c r="F95" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="82" spans="2:6">
-      <c r="B82" s="3" t="s">
+    <row r="96" spans="1:6">
+      <c r="B96" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F82" s="3">
+      <c r="F96" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="83" spans="2:6">
-      <c r="B83" s="3" t="s">
+    <row r="97" spans="2:6">
+      <c r="B97" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F83" s="3">
+      <c r="F97" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="84" spans="2:6">
-      <c r="B84" s="3" t="s">
+    <row r="98" spans="2:6">
+      <c r="B98" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="F84" s="3">
+      <c r="F98" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="85" spans="2:6">
-      <c r="B85" s="3" t="s">
+    <row r="99" spans="2:6">
+      <c r="B99" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F99" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="86" spans="2:6">
-      <c r="B86" s="3" t="s">
+    <row r="100" spans="2:6">
+      <c r="B100" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F86" s="3">
+      <c r="F100" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="87" spans="2:6">
-      <c r="B87" s="3" t="s">
+    <row r="101" spans="2:6">
+      <c r="B101" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D101" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F87" s="3">
+      <c r="F101" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="88" spans="2:6">
-      <c r="B88" s="3" t="s">
+    <row r="102" spans="2:6">
+      <c r="B102" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D102" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F88" s="3">
+      <c r="F102" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="89" spans="2:6">
-      <c r="B89" s="3" t="s">
+    <row r="103" spans="2:6">
+      <c r="B103" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D103" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F89" s="3">
+      <c r="F103" s="3">
         <v>20190204</v>
       </c>
     </row>
-    <row r="90" spans="2:6">
-      <c r="B90" s="3" t="s">
+    <row r="104" spans="2:6">
+      <c r="B104" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F90" s="3">
+      <c r="F104" s="3">
         <v>20190204</v>
       </c>
     </row>

</xml_diff>